<commit_message>
project proposal 2nd submission
</commit_message>
<xml_diff>
--- a/Capstone/Training Log.xlsx
+++ b/Capstone/Training Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="992"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>model</t>
   </si>
@@ -80,13 +80,10 @@
     <t>with inverse</t>
   </si>
   <si>
-    <t>fix up y-values in test data. Not strictly valid. - Not really such an issue. Just 1 record in 300'000 wrong</t>
-  </si>
-  <si>
-    <t>TODO:</t>
-  </si>
-  <si>
-    <t>X</t>
+    <t>repeat to check consistency</t>
+  </si>
+  <si>
+    <t>lookahead minutes</t>
   </si>
 </sst>
 </file>
@@ -406,147 +403,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.30259999999999998</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.31130000000000002</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.25700000000000001</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.17699999999999999</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>20</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.30249999999999999</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.31009999999999999</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.25800000000000001</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.17899999999999999</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>20</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.15790000000000001</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.15670000000000001</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.254</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.2001</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>0.15790000000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.15670000000000001</v>
+      </c>
+      <c r="H5">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="I5">
+        <v>0.22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>